<commit_message>
lookup fixed for studentterm records
</commit_message>
<xml_diff>
--- a/student/kogdata.xlsx
+++ b/student/kogdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheva\Desktop\dj\sms\student\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8E61E1-178E-4755-A6FD-41C91AE1670A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECF90FF-66BB-43EA-BBE8-B76F5F9B7BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1418" windowWidth="17858" windowHeight="9382" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="357">
   <si>
     <t>full_name</t>
   </si>
@@ -437,24 +437,12 @@
     <t>MH 41/9</t>
   </si>
   <si>
-    <t>Pricsla Mensah</t>
-  </si>
-  <si>
     <t xml:space="preserve">kg2 </t>
   </si>
   <si>
-    <t xml:space="preserve">Bernard Ahoto </t>
-  </si>
-  <si>
-    <t>Dunya Olivia</t>
-  </si>
-  <si>
     <t>masonry</t>
   </si>
   <si>
-    <t>MD 623/9</t>
-  </si>
-  <si>
     <t>Richiel Owusua Hammond</t>
   </si>
   <si>
@@ -1071,6 +1059,54 @@
   </si>
   <si>
     <t>Beatrice Agyemang</t>
+  </si>
+  <si>
+    <t>Felix K. Asamoah</t>
+  </si>
+  <si>
+    <t>Shantel Akosua Boakye Nyamekye</t>
+  </si>
+  <si>
+    <t>Ekua Ofori Boahene</t>
+  </si>
+  <si>
+    <t>Prince Obuakoh Okyere</t>
+  </si>
+  <si>
+    <t>Juliet Biney</t>
+  </si>
+  <si>
+    <t>Naah Shelly Tetteh</t>
+  </si>
+  <si>
+    <t>Wisdom Donkoh</t>
+  </si>
+  <si>
+    <t>Raynard Donkoh</t>
+  </si>
+  <si>
+    <t>Obrengpong Adriel</t>
+  </si>
+  <si>
+    <t>Samuel Dickson Arthur</t>
+  </si>
+  <si>
+    <t>Henry Adamtey</t>
+  </si>
+  <si>
+    <t>Anabel Mensah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kojo Prah </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg 2 </t>
+  </si>
+  <si>
+    <t>Moses Dazie</t>
+  </si>
+  <si>
+    <t>Naadom Yeboah</t>
   </si>
 </sst>
 </file>
@@ -1393,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1427,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1548,7 +1584,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -1823,10 +1859,10 @@
         <v>26</v>
       </c>
       <c r="T7">
+        <v>554246016</v>
+      </c>
+      <c r="U7">
         <v>541473757</v>
-      </c>
-      <c r="U7">
-        <v>554246016</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.45">
@@ -1834,7 +1870,7 @@
         <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -1893,7 +1929,7 @@
         <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1946,7 +1982,7 @@
         <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -2005,7 +2041,7 @@
         <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -2058,7 +2094,7 @@
         <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -2108,7 +2144,7 @@
         <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -2158,7 +2194,7 @@
         <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -2208,7 +2244,7 @@
         <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
@@ -2258,7 +2294,7 @@
         <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -2367,7 +2403,7 @@
         <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -2420,7 +2456,7 @@
         <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
@@ -2462,10 +2498,10 @@
         <v>26</v>
       </c>
       <c r="T19">
+        <v>543279537</v>
+      </c>
+      <c r="U19">
         <v>241208687</v>
-      </c>
-      <c r="U19">
-        <v>543279537</v>
       </c>
       <c r="V19" t="s">
         <v>132</v>
@@ -2473,23 +2509,20 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="1">
-        <v>43980</v>
+        <v>42673</v>
       </c>
       <c r="E20" t="s">
         <v>26</v>
       </c>
-      <c r="G20" t="s">
-        <v>134</v>
-      </c>
       <c r="H20" t="s">
         <v>37</v>
       </c>
@@ -2500,17 +2533,8 @@
         <v>21</v>
       </c>
       <c r="N20" t="s">
-        <v>135</v>
-      </c>
-      <c r="O20" t="s">
         <v>136</v>
       </c>
-      <c r="P20" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>46</v>
-      </c>
       <c r="R20" t="s">
         <v>26</v>
       </c>
@@ -2518,51 +2542,48 @@
         <v>26</v>
       </c>
       <c r="T20">
-        <v>532729761</v>
-      </c>
-      <c r="U20">
-        <v>256701567</v>
-      </c>
-      <c r="V20" t="s">
-        <v>138</v>
+        <v>244423888</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="1">
+        <v>42691</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" t="s">
+        <v>138</v>
+      </c>
+      <c r="K21" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" t="s">
         <v>139</v>
       </c>
-      <c r="B21" t="s">
-        <v>271</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="1">
-        <v>42673</v>
-      </c>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="R21" t="s">
+        <v>26</v>
+      </c>
+      <c r="S21" t="s">
+        <v>26</v>
+      </c>
+      <c r="V21" t="s">
         <v>140</v>
-      </c>
-      <c r="R21" t="s">
-        <v>26</v>
-      </c>
-      <c r="S21" t="s">
-        <v>26</v>
-      </c>
-      <c r="T21">
-        <v>244423888</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.45">
@@ -2570,31 +2591,37 @@
         <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="1">
-        <v>42691</v>
+      <c r="D22" s="2">
+        <v>42832</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
       </c>
+      <c r="G22" t="s">
+        <v>142</v>
+      </c>
       <c r="H22" t="s">
         <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="K22" t="s">
         <v>21</v>
       </c>
+      <c r="N22" t="s">
+        <v>143</v>
+      </c>
       <c r="O22" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="P22" t="s">
+        <v>146</v>
       </c>
       <c r="R22" t="s">
         <v>26</v>
@@ -2602,46 +2629,49 @@
       <c r="S22" t="s">
         <v>26</v>
       </c>
+      <c r="T22">
+        <v>245766735</v>
+      </c>
+      <c r="U22">
+        <v>245702914</v>
+      </c>
       <c r="V22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="2">
-        <v>42832</v>
+      <c r="D23" s="1">
+        <v>42202</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
       </c>
-      <c r="G23" t="s">
-        <v>146</v>
-      </c>
       <c r="H23" t="s">
         <v>37</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>101</v>
+      </c>
+      <c r="J23" t="s">
+        <v>148</v>
       </c>
       <c r="K23" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="N23" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="O23" t="s">
-        <v>148</v>
-      </c>
-      <c r="P23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R23" t="s">
         <v>26</v>
@@ -2650,42 +2680,42 @@
         <v>26</v>
       </c>
       <c r="T23">
-        <v>245766735</v>
+        <v>248178775</v>
       </c>
       <c r="U23">
-        <v>245702914</v>
+        <v>550234225</v>
       </c>
       <c r="V23" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="1">
-        <v>42202</v>
+        <v>42695</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
       </c>
+      <c r="G24" t="s">
+        <v>142</v>
+      </c>
       <c r="H24" t="s">
         <v>37</v>
       </c>
       <c r="I24" t="s">
-        <v>101</v>
-      </c>
-      <c r="J24" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="K24" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="N24" t="s">
         <v>154</v>
@@ -2693,6 +2723,12 @@
       <c r="O24" t="s">
         <v>155</v>
       </c>
+      <c r="P24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>109</v>
+      </c>
       <c r="R24" t="s">
         <v>26</v>
       </c>
@@ -2700,10 +2736,10 @@
         <v>26</v>
       </c>
       <c r="T24">
-        <v>248178775</v>
+        <v>245424585</v>
       </c>
       <c r="U24">
-        <v>550234225</v>
+        <v>247566924</v>
       </c>
       <c r="V24" t="s">
         <v>156</v>
@@ -2714,19 +2750,19 @@
         <v>157</v>
       </c>
       <c r="B25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1">
-        <v>42695</v>
+        <v>41794</v>
       </c>
       <c r="E25" t="s">
         <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="H25" t="s">
         <v>37</v>
@@ -2744,10 +2780,10 @@
         <v>159</v>
       </c>
       <c r="P25" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="Q25" t="s">
-        <v>109</v>
+        <v>160</v>
       </c>
       <c r="R25" t="s">
         <v>26</v>
@@ -2756,34 +2792,31 @@
         <v>26</v>
       </c>
       <c r="T25">
-        <v>245424585</v>
+        <v>245980902</v>
       </c>
       <c r="U25">
-        <v>247566924</v>
+        <v>245272449</v>
       </c>
       <c r="V25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1">
-        <v>41794</v>
+        <v>43093</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
       </c>
-      <c r="G26" t="s">
-        <v>112</v>
-      </c>
       <c r="H26" t="s">
         <v>37</v>
       </c>
@@ -2794,16 +2827,16 @@
         <v>21</v>
       </c>
       <c r="N26" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O26" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="P26" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="Q26" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="R26" t="s">
         <v>26</v>
@@ -2818,25 +2851,28 @@
         <v>245272449</v>
       </c>
       <c r="V26" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="1">
-        <v>43093</v>
+        <v>43165</v>
       </c>
       <c r="E27" t="s">
         <v>26</v>
       </c>
+      <c r="F27" t="s">
+        <v>164</v>
+      </c>
       <c r="H27" t="s">
         <v>37</v>
       </c>
@@ -2847,16 +2883,10 @@
         <v>21</v>
       </c>
       <c r="N27" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="O27" t="s">
-        <v>163</v>
-      </c>
-      <c r="P27" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="R27" t="s">
         <v>26</v>
@@ -2865,33 +2895,33 @@
         <v>26</v>
       </c>
       <c r="T27">
-        <v>245980902</v>
+        <v>543784758</v>
       </c>
       <c r="U27">
-        <v>245272449</v>
+        <v>243307643</v>
       </c>
       <c r="V27" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C28" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="1">
-        <v>43165</v>
+        <v>42564</v>
       </c>
       <c r="E28" t="s">
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H28" t="s">
         <v>37</v>
@@ -2899,14 +2929,17 @@
       <c r="I28" t="s">
         <v>21</v>
       </c>
+      <c r="J28" t="s">
+        <v>169</v>
+      </c>
       <c r="K28" t="s">
         <v>21</v>
       </c>
       <c r="N28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="O28" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R28" t="s">
         <v>26</v>
@@ -2921,27 +2954,27 @@
         <v>243307643</v>
       </c>
       <c r="V28" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B29" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="1">
-        <v>42564</v>
+        <v>43499</v>
       </c>
       <c r="E29" t="s">
         <v>26</v>
       </c>
       <c r="F29" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
@@ -2949,17 +2982,20 @@
       <c r="I29" t="s">
         <v>21</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" t="s">
+        <v>172</v>
+      </c>
+      <c r="O29" t="s">
         <v>173</v>
       </c>
-      <c r="K29" t="s">
-        <v>21</v>
-      </c>
-      <c r="N29" t="s">
-        <v>169</v>
-      </c>
-      <c r="O29" t="s">
-        <v>170</v>
+      <c r="P29" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>25</v>
       </c>
       <c r="R29" t="s">
         <v>26</v>
@@ -2968,33 +3004,33 @@
         <v>26</v>
       </c>
       <c r="T29">
-        <v>543784758</v>
+        <v>595670927</v>
       </c>
       <c r="U29">
-        <v>243307643</v>
+        <v>553491903</v>
       </c>
       <c r="V29" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="1">
-        <v>43499</v>
+        <v>42289</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
       </c>
-      <c r="F30" t="s">
-        <v>175</v>
+      <c r="G30" t="s">
+        <v>122</v>
       </c>
       <c r="H30" t="s">
         <v>37</v>
@@ -3012,10 +3048,10 @@
         <v>177</v>
       </c>
       <c r="P30" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="Q30" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="R30" t="s">
         <v>26</v>
@@ -3024,34 +3060,31 @@
         <v>26</v>
       </c>
       <c r="T30">
-        <v>595670927</v>
+        <v>547068449</v>
       </c>
       <c r="U30">
-        <v>553491903</v>
+        <v>547068449</v>
       </c>
       <c r="V30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B31" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D31" s="1">
-        <v>42289</v>
+        <v>42839</v>
       </c>
       <c r="E31" t="s">
         <v>26</v>
       </c>
-      <c r="G31" t="s">
-        <v>122</v>
-      </c>
       <c r="H31" t="s">
         <v>37</v>
       </c>
@@ -3062,17 +3095,11 @@
         <v>21</v>
       </c>
       <c r="N31" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="O31" t="s">
-        <v>181</v>
-      </c>
-      <c r="P31" t="s">
         <v>182</v>
       </c>
-      <c r="Q31" t="s">
-        <v>109</v>
-      </c>
       <c r="R31" t="s">
         <v>26</v>
       </c>
@@ -3080,10 +3107,10 @@
         <v>26</v>
       </c>
       <c r="T31">
-        <v>547068449</v>
+        <v>244730682</v>
       </c>
       <c r="U31">
-        <v>547068449</v>
+        <v>249341294</v>
       </c>
       <c r="V31" t="s">
         <v>183</v>
@@ -3094,31 +3121,49 @@
         <v>184</v>
       </c>
       <c r="B32" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="1">
-        <v>42839</v>
+        <v>44495</v>
       </c>
       <c r="E32" t="s">
         <v>26</v>
       </c>
+      <c r="F32" t="s">
+        <v>185</v>
+      </c>
+      <c r="G32" t="s">
+        <v>122</v>
+      </c>
       <c r="H32" t="s">
         <v>37</v>
       </c>
       <c r="I32" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="J32" t="s">
+        <v>186</v>
       </c>
       <c r="K32" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="L32" t="s">
+        <v>187</v>
       </c>
       <c r="N32" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="O32" t="s">
-        <v>186</v>
+        <v>189</v>
+      </c>
+      <c r="P32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>190</v>
       </c>
       <c r="R32" t="s">
         <v>26</v>
@@ -3127,63 +3172,60 @@
         <v>26</v>
       </c>
       <c r="T32">
-        <v>244730682</v>
+        <v>532416380</v>
       </c>
       <c r="U32">
-        <v>249341294</v>
+        <v>543108512</v>
       </c>
       <c r="V32" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B33" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D33" s="1">
-        <v>44495</v>
+        <v>43950</v>
       </c>
       <c r="E33" t="s">
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G33" t="s">
-        <v>122</v>
+        <v>36</v>
       </c>
       <c r="H33" t="s">
         <v>37</v>
       </c>
       <c r="I33" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="J33" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="K33" t="s">
-        <v>37</v>
-      </c>
-      <c r="L33" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
       <c r="N33" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="O33" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="P33" t="s">
-        <v>24</v>
+        <v>197</v>
       </c>
       <c r="Q33" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="R33" t="s">
         <v>26</v>
@@ -3192,93 +3234,90 @@
         <v>26</v>
       </c>
       <c r="T33">
-        <v>532416380</v>
+        <v>597661016</v>
       </c>
       <c r="U33">
-        <v>543108512</v>
+        <v>501213049</v>
       </c>
       <c r="V33" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B34" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D34" s="1">
-        <v>43950</v>
+        <v>44383</v>
       </c>
       <c r="E34" t="s">
         <v>26</v>
       </c>
-      <c r="F34" t="s">
-        <v>197</v>
-      </c>
-      <c r="G34" t="s">
-        <v>36</v>
-      </c>
       <c r="H34" t="s">
         <v>37</v>
       </c>
       <c r="I34" t="s">
-        <v>101</v>
-      </c>
-      <c r="J34" t="s">
-        <v>198</v>
+        <v>21</v>
       </c>
       <c r="K34" t="s">
         <v>21</v>
       </c>
       <c r="N34" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="O34" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="P34" t="s">
-        <v>201</v>
+        <v>40</v>
       </c>
       <c r="Q34" t="s">
+        <v>25</v>
+      </c>
+      <c r="R34" t="s">
+        <v>26</v>
+      </c>
+      <c r="S34" t="s">
+        <v>26</v>
+      </c>
+      <c r="T34">
+        <v>595670927</v>
+      </c>
+      <c r="U34">
+        <v>553491903</v>
+      </c>
+      <c r="V34" t="s">
         <v>202</v>
-      </c>
-      <c r="R34" t="s">
-        <v>26</v>
-      </c>
-      <c r="S34" t="s">
-        <v>26</v>
-      </c>
-      <c r="T34">
-        <v>597661016</v>
-      </c>
-      <c r="U34">
-        <v>501213049</v>
-      </c>
-      <c r="V34" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B35" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C35" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="1">
-        <v>44383</v>
+        <v>43524</v>
       </c>
       <c r="E35" t="s">
         <v>26</v>
       </c>
+      <c r="F35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G35" t="s">
+        <v>133</v>
+      </c>
       <c r="H35" t="s">
         <v>37</v>
       </c>
@@ -3289,16 +3328,16 @@
         <v>21</v>
       </c>
       <c r="N35" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="O35" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="P35" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
       <c r="Q35" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
       <c r="R35" t="s">
         <v>26</v>
@@ -3307,36 +3346,33 @@
         <v>26</v>
       </c>
       <c r="T35">
-        <v>595670927</v>
+        <v>244678226</v>
       </c>
       <c r="U35">
-        <v>553491903</v>
+        <v>208455305</v>
       </c>
       <c r="V35" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B36" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D36" s="1">
-        <v>43524</v>
+        <v>44364</v>
       </c>
       <c r="E36" t="s">
         <v>26</v>
       </c>
-      <c r="F36" t="s">
-        <v>208</v>
-      </c>
       <c r="G36" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="H36" t="s">
         <v>37</v>
@@ -3348,16 +3384,16 @@
         <v>21</v>
       </c>
       <c r="N36" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O36" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="P36" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="Q36" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="R36" t="s">
         <v>26</v>
@@ -3366,27 +3402,27 @@
         <v>26</v>
       </c>
       <c r="T36">
-        <v>244678226</v>
+        <v>243352028</v>
       </c>
       <c r="U36">
-        <v>208455305</v>
+        <v>243088742</v>
       </c>
       <c r="V36" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B37" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="1">
-        <v>44364</v>
+        <v>44627</v>
       </c>
       <c r="E37" t="s">
         <v>26</v>
@@ -3400,76 +3436,76 @@
       <c r="I37" t="s">
         <v>21</v>
       </c>
-      <c r="K37" t="s">
-        <v>21</v>
+      <c r="M37" t="s">
+        <v>216</v>
       </c>
       <c r="N37" t="s">
-        <v>214</v>
+        <v>79</v>
       </c>
       <c r="O37" t="s">
-        <v>215</v>
+        <v>80</v>
       </c>
       <c r="P37" t="s">
-        <v>216</v>
+        <v>24</v>
       </c>
       <c r="Q37" t="s">
+        <v>82</v>
+      </c>
+      <c r="R37" t="s">
+        <v>26</v>
+      </c>
+      <c r="S37" t="s">
+        <v>26</v>
+      </c>
+      <c r="T37">
+        <v>241861382</v>
+      </c>
+      <c r="U37">
+        <v>547944747</v>
+      </c>
+      <c r="V37" t="s">
         <v>217</v>
-      </c>
-      <c r="R37" t="s">
-        <v>26</v>
-      </c>
-      <c r="S37" t="s">
-        <v>26</v>
-      </c>
-      <c r="T37">
-        <v>243352028</v>
-      </c>
-      <c r="U37">
-        <v>243088742</v>
-      </c>
-      <c r="V37" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>218</v>
+      </c>
+      <c r="B38" t="s">
+        <v>264</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="1">
+        <v>44430</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" t="s">
+        <v>96</v>
+      </c>
+      <c r="H38" t="s">
+        <v>37</v>
+      </c>
+      <c r="I38" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" t="s">
+        <v>21</v>
+      </c>
+      <c r="N38" t="s">
         <v>219</v>
       </c>
-      <c r="B38" t="s">
-        <v>267</v>
-      </c>
-      <c r="C38" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="1">
-        <v>44627</v>
-      </c>
-      <c r="E38" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" t="s">
-        <v>122</v>
-      </c>
-      <c r="H38" t="s">
-        <v>37</v>
-      </c>
-      <c r="I38" t="s">
-        <v>21</v>
-      </c>
-      <c r="M38" t="s">
+      <c r="O38" t="s">
         <v>220</v>
       </c>
-      <c r="N38" t="s">
-        <v>79</v>
-      </c>
-      <c r="O38" t="s">
-        <v>80</v>
-      </c>
       <c r="P38" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="Q38" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
       <c r="R38" t="s">
         <v>26</v>
@@ -3478,54 +3514,54 @@
         <v>26</v>
       </c>
       <c r="T38">
-        <v>241861382</v>
+        <v>555101040</v>
       </c>
       <c r="U38">
-        <v>547944747</v>
+        <v>537150359</v>
       </c>
       <c r="V38" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="B39" t="s">
         <v>268</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D39" s="1">
-        <v>44430</v>
+        <v>43839</v>
       </c>
       <c r="E39" t="s">
         <v>26</v>
+      </c>
+      <c r="F39" t="s">
+        <v>223</v>
       </c>
       <c r="G39" t="s">
         <v>96</v>
       </c>
       <c r="H39" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="I39" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="J39" t="s">
+        <v>224</v>
       </c>
       <c r="K39" t="s">
         <v>21</v>
       </c>
       <c r="N39" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="O39" t="s">
-        <v>224</v>
-      </c>
-      <c r="P39" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="R39" t="s">
         <v>26</v>
@@ -3534,90 +3570,87 @@
         <v>26</v>
       </c>
       <c r="T39">
-        <v>555101040</v>
+        <v>554845413</v>
       </c>
       <c r="U39">
-        <v>537150359</v>
+        <v>256786281</v>
       </c>
       <c r="V39" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="B40" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
       </c>
       <c r="D40" s="1">
-        <v>43839</v>
+        <v>44661</v>
       </c>
       <c r="E40" t="s">
         <v>26</v>
-      </c>
-      <c r="F40" t="s">
-        <v>227</v>
       </c>
       <c r="G40" t="s">
         <v>96</v>
       </c>
       <c r="H40" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="I40" t="s">
-        <v>37</v>
-      </c>
-      <c r="J40" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
       <c r="K40" t="s">
         <v>21</v>
       </c>
       <c r="N40" t="s">
+        <v>154</v>
+      </c>
+      <c r="O40" t="s">
+        <v>155</v>
+      </c>
+      <c r="P40" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>25</v>
+      </c>
+      <c r="R40" t="s">
+        <v>26</v>
+      </c>
+      <c r="S40" t="s">
+        <v>26</v>
+      </c>
+      <c r="T40">
+        <v>245424585</v>
+      </c>
+      <c r="U40">
+        <v>247566924</v>
+      </c>
+      <c r="V40" t="s">
         <v>229</v>
-      </c>
-      <c r="O40" t="s">
-        <v>230</v>
-      </c>
-      <c r="R40" t="s">
-        <v>26</v>
-      </c>
-      <c r="S40" t="s">
-        <v>26</v>
-      </c>
-      <c r="T40">
-        <v>554845413</v>
-      </c>
-      <c r="U40">
-        <v>256786281</v>
-      </c>
-      <c r="V40" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B41" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="1">
-        <v>44661</v>
+        <v>44459</v>
       </c>
       <c r="E41" t="s">
         <v>26</v>
       </c>
-      <c r="G41" t="s">
-        <v>96</v>
-      </c>
       <c r="H41" t="s">
         <v>37</v>
       </c>
@@ -3628,16 +3661,13 @@
         <v>21</v>
       </c>
       <c r="N41" t="s">
-        <v>158</v>
+        <v>231</v>
       </c>
       <c r="O41" t="s">
-        <v>159</v>
+        <v>232</v>
       </c>
       <c r="P41" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>25</v>
+        <v>233</v>
       </c>
       <c r="R41" t="s">
         <v>26</v>
@@ -3646,13 +3676,13 @@
         <v>26</v>
       </c>
       <c r="T41">
-        <v>245424585</v>
+        <v>244446781</v>
       </c>
       <c r="U41">
-        <v>247566924</v>
+        <v>249251741</v>
       </c>
       <c r="V41" t="s">
-        <v>233</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.45">
@@ -3660,13 +3690,13 @@
         <v>234</v>
       </c>
       <c r="B42" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D42" s="1">
-        <v>44459</v>
+        <v>44414</v>
       </c>
       <c r="E42" t="s">
         <v>26</v>
@@ -3689,6 +3719,9 @@
       <c r="P42" t="s">
         <v>237</v>
       </c>
+      <c r="Q42" t="s">
+        <v>237</v>
+      </c>
       <c r="R42" t="s">
         <v>26</v>
       </c>
@@ -3696,13 +3729,13 @@
         <v>26</v>
       </c>
       <c r="T42">
-        <v>244446781</v>
+        <v>246364382</v>
       </c>
       <c r="U42">
-        <v>249251741</v>
+        <v>242830458</v>
       </c>
       <c r="V42" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.45">
@@ -3710,22 +3743,28 @@
         <v>238</v>
       </c>
       <c r="B43" t="s">
-        <v>273</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="1">
-        <v>44414</v>
+        <v>45025</v>
       </c>
       <c r="E43" t="s">
         <v>26</v>
       </c>
+      <c r="G43" t="s">
+        <v>122</v>
+      </c>
       <c r="H43" t="s">
         <v>37</v>
       </c>
       <c r="I43" t="s">
         <v>21</v>
+      </c>
+      <c r="J43" t="s">
+        <v>169</v>
       </c>
       <c r="K43" t="s">
         <v>21</v>
@@ -3740,7 +3779,7 @@
         <v>241</v>
       </c>
       <c r="Q43" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="R43" t="s">
         <v>26</v>
@@ -3749,57 +3788,54 @@
         <v>26</v>
       </c>
       <c r="T43">
-        <v>246364382</v>
+        <v>245902055</v>
       </c>
       <c r="U43">
-        <v>242830458</v>
-      </c>
-      <c r="V43" t="s">
-        <v>165</v>
+        <v>557566068</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>269</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D44" s="1">
-        <v>45025</v>
+        <v>43792</v>
       </c>
       <c r="E44" t="s">
         <v>26</v>
       </c>
-      <c r="G44" t="s">
-        <v>122</v>
+      <c r="F44" t="s">
+        <v>244</v>
       </c>
       <c r="H44" t="s">
         <v>37</v>
       </c>
       <c r="I44" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="J44" t="s">
-        <v>173</v>
+        <v>245</v>
       </c>
       <c r="K44" t="s">
         <v>21</v>
       </c>
       <c r="N44" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O44" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="P44" t="s">
-        <v>245</v>
+        <v>40</v>
       </c>
       <c r="Q44" t="s">
-        <v>246</v>
+        <v>25</v>
       </c>
       <c r="R44" t="s">
         <v>26</v>
@@ -3808,51 +3844,54 @@
         <v>26</v>
       </c>
       <c r="T44">
-        <v>245902055</v>
+        <v>538984324</v>
       </c>
       <c r="U44">
-        <v>557566068</v>
+        <v>531766425</v>
+      </c>
+      <c r="V44" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B45" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D45" s="1">
-        <v>43792</v>
+        <v>43785</v>
       </c>
       <c r="E45" t="s">
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>248</v>
+        <v>250</v>
+      </c>
+      <c r="G45" t="s">
+        <v>133</v>
       </c>
       <c r="H45" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="I45" t="s">
-        <v>37</v>
-      </c>
-      <c r="J45" t="s">
-        <v>249</v>
+        <v>21</v>
       </c>
       <c r="K45" t="s">
         <v>21</v>
       </c>
       <c r="N45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O45" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P45" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="Q45" t="s">
         <v>25</v>
@@ -3864,13 +3903,10 @@
         <v>26</v>
       </c>
       <c r="T45">
-        <v>538984324</v>
+        <v>549821786</v>
       </c>
       <c r="U45">
-        <v>531766425</v>
-      </c>
-      <c r="V45" t="s">
-        <v>252</v>
+        <v>256242568</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.45">
@@ -3878,25 +3914,22 @@
         <v>253</v>
       </c>
       <c r="B46" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C46" t="s">
         <v>20</v>
       </c>
       <c r="D46" s="1">
-        <v>43785</v>
+        <v>44687</v>
       </c>
       <c r="E46" t="s">
         <v>26</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
+        <v>96</v>
+      </c>
+      <c r="H46" t="s">
         <v>254</v>
-      </c>
-      <c r="G46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H46" t="s">
-        <v>21</v>
       </c>
       <c r="I46" t="s">
         <v>21</v>
@@ -3910,12 +3943,6 @@
       <c r="O46" t="s">
         <v>256</v>
       </c>
-      <c r="P46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>25</v>
-      </c>
       <c r="R46" t="s">
         <v>26</v>
       </c>
@@ -3923,45 +3950,60 @@
         <v>26</v>
       </c>
       <c r="T46">
-        <v>549821786</v>
+        <v>247633503</v>
       </c>
       <c r="U46">
-        <v>256242568</v>
+        <v>241690416</v>
+      </c>
+      <c r="V46" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B47" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C47" t="s">
         <v>20</v>
       </c>
       <c r="D47" s="1">
-        <v>44687</v>
+        <v>42797</v>
       </c>
       <c r="E47" t="s">
         <v>26</v>
       </c>
+      <c r="F47" t="s">
+        <v>244</v>
+      </c>
       <c r="G47" t="s">
-        <v>96</v>
+        <v>259</v>
       </c>
       <c r="H47" t="s">
-        <v>258</v>
+        <v>21</v>
       </c>
       <c r="I47" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="J47" t="s">
+        <v>245</v>
       </c>
       <c r="K47" t="s">
         <v>21</v>
       </c>
       <c r="N47" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="O47" t="s">
-        <v>260</v>
+        <v>247</v>
+      </c>
+      <c r="P47" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>25</v>
       </c>
       <c r="R47" t="s">
         <v>26</v>
@@ -3970,18 +4012,18 @@
         <v>26</v>
       </c>
       <c r="T47">
-        <v>247633503</v>
+        <v>538984324</v>
       </c>
       <c r="U47">
-        <v>241690416</v>
+        <v>531766425</v>
       </c>
       <c r="V47" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B48" t="s">
         <v>263</v>
@@ -3990,34 +4032,28 @@
         <v>20</v>
       </c>
       <c r="D48" s="1">
-        <v>42797</v>
+        <v>44663</v>
       </c>
       <c r="E48" t="s">
         <v>26</v>
       </c>
-      <c r="F48" t="s">
-        <v>248</v>
-      </c>
       <c r="G48" t="s">
-        <v>263</v>
+        <v>96</v>
       </c>
       <c r="H48" t="s">
         <v>21</v>
       </c>
       <c r="I48" t="s">
-        <v>37</v>
-      </c>
-      <c r="J48" t="s">
-        <v>249</v>
+        <v>149</v>
       </c>
       <c r="K48" t="s">
         <v>21</v>
       </c>
       <c r="N48" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="O48" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="P48" t="s">
         <v>40</v>
@@ -4038,48 +4074,54 @@
         <v>531766425</v>
       </c>
       <c r="V48" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="B49" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D49" s="1">
-        <v>44663</v>
+        <v>42239</v>
       </c>
       <c r="E49" t="s">
         <v>26</v>
       </c>
-      <c r="G49" t="s">
-        <v>96</v>
+      <c r="F49" t="s">
+        <v>272</v>
       </c>
       <c r="H49" t="s">
         <v>21</v>
       </c>
       <c r="I49" t="s">
-        <v>153</v>
+        <v>101</v>
+      </c>
+      <c r="J49" t="s">
+        <v>279</v>
       </c>
       <c r="K49" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="L49" t="s">
+        <v>273</v>
       </c>
       <c r="N49" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="O49" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="P49" t="s">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="Q49" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="R49" t="s">
         <v>26</v>
@@ -4088,57 +4130,48 @@
         <v>26</v>
       </c>
       <c r="T49">
-        <v>538984324</v>
+        <v>549605899</v>
       </c>
       <c r="U49">
-        <v>531766425</v>
-      </c>
-      <c r="V49" t="s">
-        <v>252</v>
+        <v>534014247</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C50" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="1">
-        <v>42239</v>
+        <v>43231</v>
       </c>
       <c r="E50" t="s">
         <v>26</v>
       </c>
-      <c r="F50" t="s">
-        <v>276</v>
-      </c>
       <c r="H50" t="s">
         <v>21</v>
       </c>
       <c r="I50" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="J50" t="s">
-        <v>283</v>
+        <v>138</v>
       </c>
       <c r="K50" t="s">
-        <v>37</v>
-      </c>
-      <c r="L50" t="s">
-        <v>277</v>
+        <v>21</v>
       </c>
       <c r="N50" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="O50" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="P50" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="Q50" t="s">
         <v>109</v>
@@ -4150,48 +4183,51 @@
         <v>26</v>
       </c>
       <c r="T50">
-        <v>549605899</v>
+        <v>244077227</v>
       </c>
       <c r="U50">
-        <v>534014247</v>
+        <v>245173168</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B51" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C51" t="s">
         <v>34</v>
       </c>
       <c r="D51" s="1">
-        <v>43231</v>
+        <v>42088</v>
       </c>
       <c r="E51" t="s">
         <v>26</v>
       </c>
       <c r="H51" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="I51" t="s">
         <v>37</v>
       </c>
       <c r="J51" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K51" t="s">
-        <v>21</v>
+        <v>101</v>
+      </c>
+      <c r="L51" t="s">
+        <v>280</v>
       </c>
       <c r="N51" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="O51" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="P51" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="Q51" t="s">
         <v>109</v>
@@ -4203,51 +4239,51 @@
         <v>26</v>
       </c>
       <c r="T51">
-        <v>244077227</v>
+        <v>207900244</v>
       </c>
       <c r="U51">
-        <v>245173168</v>
+        <v>599397215</v>
+      </c>
+      <c r="V51" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B52" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D52" s="1">
-        <v>42088</v>
+        <v>43085</v>
       </c>
       <c r="E52" t="s">
         <v>26</v>
       </c>
       <c r="H52" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="I52" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="J52" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="K52" t="s">
-        <v>101</v>
-      </c>
-      <c r="L52" t="s">
-        <v>284</v>
+        <v>21</v>
       </c>
       <c r="N52" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="O52" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="P52" t="s">
-        <v>287</v>
+        <v>109</v>
       </c>
       <c r="Q52" t="s">
         <v>109</v>
@@ -4259,27 +4295,24 @@
         <v>26</v>
       </c>
       <c r="T52">
-        <v>207900244</v>
+        <v>243043900</v>
       </c>
       <c r="U52">
-        <v>599397215</v>
-      </c>
-      <c r="V52" t="s">
-        <v>288</v>
+        <v>549370765</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B53" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C53" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="1">
-        <v>43085</v>
+        <v>43108</v>
       </c>
       <c r="E53" t="s">
         <v>26</v>
@@ -4288,25 +4321,22 @@
         <v>21</v>
       </c>
       <c r="I53" t="s">
-        <v>21</v>
-      </c>
-      <c r="J53" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="K53" t="s">
         <v>21</v>
       </c>
       <c r="N53" t="s">
+        <v>292</v>
+      </c>
+      <c r="O53" t="s">
         <v>293</v>
       </c>
-      <c r="O53" t="s">
+      <c r="P53" t="s">
         <v>294</v>
       </c>
-      <c r="P53" t="s">
-        <v>109</v>
-      </c>
       <c r="Q53" t="s">
-        <v>109</v>
+        <v>213</v>
       </c>
       <c r="R53" t="s">
         <v>26</v>
@@ -4315,10 +4345,10 @@
         <v>26</v>
       </c>
       <c r="T53">
-        <v>243043900</v>
+        <v>533254698</v>
       </c>
       <c r="U53">
-        <v>549370765</v>
+        <v>546589599</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.45">
@@ -4326,22 +4356,25 @@
         <v>295</v>
       </c>
       <c r="B54" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C54" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="1">
-        <v>43108</v>
+        <v>43310</v>
       </c>
       <c r="E54" t="s">
         <v>26</v>
       </c>
+      <c r="F54" t="s">
+        <v>111</v>
+      </c>
       <c r="H54" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="I54" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K54" t="s">
         <v>21</v>
@@ -4353,22 +4386,25 @@
         <v>297</v>
       </c>
       <c r="P54" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>25</v>
+      </c>
+      <c r="R54" t="s">
+        <v>26</v>
+      </c>
+      <c r="S54" t="s">
+        <v>26</v>
+      </c>
+      <c r="T54">
+        <v>249220522</v>
+      </c>
+      <c r="U54">
+        <v>241246842</v>
+      </c>
+      <c r="V54" t="s">
         <v>298</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>217</v>
-      </c>
-      <c r="R54" t="s">
-        <v>26</v>
-      </c>
-      <c r="S54" t="s">
-        <v>26</v>
-      </c>
-      <c r="T54">
-        <v>533254698</v>
-      </c>
-      <c r="U54">
-        <v>546589599</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.45">
@@ -4376,40 +4412,40 @@
         <v>299</v>
       </c>
       <c r="B55" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C55" t="s">
         <v>20</v>
       </c>
       <c r="D55" s="1">
-        <v>43310</v>
+        <v>43170</v>
       </c>
       <c r="E55" t="s">
         <v>26</v>
       </c>
-      <c r="F55" t="s">
-        <v>111</v>
-      </c>
       <c r="H55" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="I55" t="s">
-        <v>153</v>
+        <v>37</v>
+      </c>
+      <c r="J55" t="s">
+        <v>300</v>
       </c>
       <c r="K55" t="s">
         <v>21</v>
       </c>
       <c r="N55" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O55" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P55" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="Q55" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="R55" t="s">
         <v>26</v>
@@ -4418,13 +4454,10 @@
         <v>26</v>
       </c>
       <c r="T55">
-        <v>249220522</v>
+        <v>246861527</v>
       </c>
       <c r="U55">
-        <v>241246842</v>
-      </c>
-      <c r="V55" t="s">
-        <v>302</v>
+        <v>558286552</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.45">
@@ -4432,40 +4465,40 @@
         <v>303</v>
       </c>
       <c r="B56" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D56" s="1">
-        <v>43170</v>
+        <v>43452</v>
       </c>
       <c r="E56" t="s">
         <v>26</v>
       </c>
       <c r="H56" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="I56" t="s">
         <v>37</v>
       </c>
       <c r="J56" t="s">
+        <v>138</v>
+      </c>
+      <c r="K56" t="s">
+        <v>149</v>
+      </c>
+      <c r="N56" t="s">
         <v>304</v>
       </c>
-      <c r="K56" t="s">
-        <v>21</v>
-      </c>
-      <c r="N56" t="s">
+      <c r="O56" t="s">
         <v>305</v>
       </c>
-      <c r="O56" t="s">
+      <c r="P56" t="s">
         <v>306</v>
       </c>
-      <c r="P56" t="s">
-        <v>137</v>
-      </c>
       <c r="Q56" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="R56" t="s">
         <v>26</v>
@@ -4474,24 +4507,27 @@
         <v>26</v>
       </c>
       <c r="T56">
-        <v>246861527</v>
+        <v>246532233</v>
       </c>
       <c r="U56">
-        <v>558286552</v>
+        <v>247792191</v>
+      </c>
+      <c r="V56" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B57" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C57" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="1">
-        <v>43452</v>
+        <v>43118</v>
       </c>
       <c r="E57" t="s">
         <v>26</v>
@@ -4500,78 +4536,75 @@
         <v>37</v>
       </c>
       <c r="I57" t="s">
-        <v>37</v>
-      </c>
-      <c r="J57" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="K57" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="N57" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="O57" t="s">
+        <v>314</v>
+      </c>
+      <c r="P57" t="s">
         <v>309</v>
       </c>
-      <c r="P57" t="s">
+      <c r="Q57" t="s">
+        <v>109</v>
+      </c>
+      <c r="R57" t="s">
+        <v>26</v>
+      </c>
+      <c r="S57" t="s">
+        <v>26</v>
+      </c>
+      <c r="T57">
+        <v>246951455</v>
+      </c>
+      <c r="U57">
+        <v>242684572</v>
+      </c>
+      <c r="V57" t="s">
         <v>310</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>25</v>
-      </c>
-      <c r="R57" t="s">
-        <v>26</v>
-      </c>
-      <c r="S57" t="s">
-        <v>26</v>
-      </c>
-      <c r="T57">
-        <v>246532233</v>
-      </c>
-      <c r="U57">
-        <v>247792191</v>
-      </c>
-      <c r="V57" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B58" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C58" t="s">
         <v>34</v>
       </c>
       <c r="D58" s="1">
-        <v>43118</v>
+        <v>43008</v>
       </c>
       <c r="E58" t="s">
         <v>26</v>
       </c>
+      <c r="F58" t="s">
+        <v>312</v>
+      </c>
       <c r="H58" t="s">
         <v>37</v>
       </c>
       <c r="I58" t="s">
         <v>21</v>
       </c>
-      <c r="K58" t="s">
-        <v>21</v>
-      </c>
       <c r="N58" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="O58" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="P58" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="Q58" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="R58" t="s">
         <v>26</v>
@@ -4586,27 +4619,27 @@
         <v>242684572</v>
       </c>
       <c r="V58" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s">
-        <v>269</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="1">
-        <v>43008</v>
+        <v>44912</v>
       </c>
       <c r="E59" t="s">
         <v>26</v>
       </c>
       <c r="F59" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H59" t="s">
         <v>37</v>
@@ -4615,13 +4648,13 @@
         <v>21</v>
       </c>
       <c r="N59" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="O59" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="P59" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="Q59" t="s">
         <v>25</v>
@@ -4639,45 +4672,48 @@
         <v>242684572</v>
       </c>
       <c r="V59" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
+        <v>317</v>
+      </c>
+      <c r="B60" t="s">
+        <v>318</v>
+      </c>
+      <c r="C60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="1">
+        <v>42540</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" t="s">
+        <v>319</v>
+      </c>
+      <c r="H60" t="s">
+        <v>37</v>
+      </c>
+      <c r="I60" t="s">
+        <v>21</v>
+      </c>
+      <c r="K60" t="s">
+        <v>21</v>
+      </c>
+      <c r="N60" t="s">
         <v>320</v>
       </c>
-      <c r="B60" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="1">
-        <v>44912</v>
-      </c>
-      <c r="E60" t="s">
-        <v>26</v>
-      </c>
-      <c r="F60" t="s">
-        <v>316</v>
-      </c>
-      <c r="H60" t="s">
-        <v>37</v>
-      </c>
-      <c r="I60" t="s">
-        <v>21</v>
-      </c>
-      <c r="N60" t="s">
-        <v>317</v>
-      </c>
       <c r="O60" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="P60" t="s">
-        <v>319</v>
+        <v>146</v>
       </c>
       <c r="Q60" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="R60" t="s">
         <v>26</v>
@@ -4686,34 +4722,31 @@
         <v>26</v>
       </c>
       <c r="T60">
-        <v>246951455</v>
+        <v>549223419</v>
       </c>
       <c r="U60">
-        <v>242684572</v>
+        <v>547981198</v>
       </c>
       <c r="V60" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B61" t="s">
-        <v>322</v>
+        <v>263</v>
       </c>
       <c r="C61" t="s">
         <v>20</v>
       </c>
       <c r="D61" s="1">
-        <v>42540</v>
+        <v>44839</v>
       </c>
       <c r="E61" t="s">
         <v>26</v>
       </c>
-      <c r="F61" t="s">
-        <v>323</v>
-      </c>
       <c r="H61" t="s">
         <v>37</v>
       </c>
@@ -4724,51 +4757,51 @@
         <v>21</v>
       </c>
       <c r="N61" t="s">
+        <v>296</v>
+      </c>
+      <c r="O61" t="s">
+        <v>297</v>
+      </c>
+      <c r="P61" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>109</v>
+      </c>
+      <c r="R61" t="s">
+        <v>26</v>
+      </c>
+      <c r="S61" t="s">
+        <v>26</v>
+      </c>
+      <c r="T61">
+        <v>249220522</v>
+      </c>
+      <c r="U61">
+        <v>241246842</v>
+      </c>
+      <c r="V61" t="s">
         <v>324</v>
-      </c>
-      <c r="O61" t="s">
-        <v>325</v>
-      </c>
-      <c r="P61" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>150</v>
-      </c>
-      <c r="R61" t="s">
-        <v>26</v>
-      </c>
-      <c r="S61" t="s">
-        <v>26</v>
-      </c>
-      <c r="T61">
-        <v>549223419</v>
-      </c>
-      <c r="U61">
-        <v>547981198</v>
-      </c>
-      <c r="V61" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C62" t="s">
         <v>20</v>
       </c>
       <c r="D62" s="1">
-        <v>44839</v>
+        <v>43831</v>
       </c>
       <c r="E62" t="s">
         <v>26</v>
       </c>
       <c r="H62" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="I62" t="s">
         <v>21</v>
@@ -4777,16 +4810,16 @@
         <v>21</v>
       </c>
       <c r="N62" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="O62" t="s">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="P62" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="Q62" t="s">
-        <v>109</v>
+        <v>328</v>
       </c>
       <c r="R62" t="s">
         <v>26</v>
@@ -4795,51 +4828,57 @@
         <v>26</v>
       </c>
       <c r="T62">
-        <v>249220522</v>
+        <v>248076761</v>
       </c>
       <c r="U62">
-        <v>241246842</v>
+        <v>551424325</v>
       </c>
       <c r="V62" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B63" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C63" t="s">
         <v>20</v>
       </c>
       <c r="D63" s="1">
-        <v>43831</v>
+        <v>44017</v>
       </c>
       <c r="E63" t="s">
         <v>26</v>
       </c>
+      <c r="F63" t="s">
+        <v>63</v>
+      </c>
       <c r="H63" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="I63" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="J63" t="s">
+        <v>331</v>
       </c>
       <c r="K63" t="s">
         <v>21</v>
       </c>
       <c r="N63" t="s">
-        <v>330</v>
+        <v>231</v>
       </c>
       <c r="O63" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="P63" t="s">
-        <v>40</v>
+        <v>233</v>
       </c>
       <c r="Q63" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="R63" t="s">
         <v>26</v>
@@ -4848,56 +4887,35 @@
         <v>26</v>
       </c>
       <c r="T63">
-        <v>248076761</v>
+        <v>244446781</v>
       </c>
       <c r="U63">
-        <v>551424325</v>
+        <v>249251741</v>
       </c>
       <c r="V63" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B64" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C64" t="s">
         <v>20</v>
       </c>
       <c r="D64" s="1">
-        <v>44017</v>
+        <v>43774</v>
       </c>
       <c r="E64" t="s">
         <v>26</v>
       </c>
-      <c r="F64" t="s">
-        <v>63</v>
-      </c>
-      <c r="H64" t="s">
-        <v>37</v>
-      </c>
-      <c r="I64" t="s">
-        <v>37</v>
-      </c>
-      <c r="J64" t="s">
-        <v>335</v>
-      </c>
-      <c r="K64" t="s">
-        <v>21</v>
-      </c>
       <c r="N64" t="s">
-        <v>235</v>
+        <v>336</v>
       </c>
       <c r="O64" t="s">
-        <v>336</v>
-      </c>
-      <c r="P64" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q64" t="s">
         <v>337</v>
       </c>
       <c r="R64" t="s">
@@ -4907,36 +4925,45 @@
         <v>26</v>
       </c>
       <c r="T64">
-        <v>244446781</v>
+        <v>242715514</v>
       </c>
       <c r="U64">
-        <v>249251741</v>
-      </c>
-      <c r="V64" t="s">
-        <v>338</v>
+        <v>553488520</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
+        <v>338</v>
+      </c>
+      <c r="B65" t="s">
+        <v>269</v>
+      </c>
+      <c r="C65" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" s="1">
+        <v>44112</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
+        <v>319</v>
+      </c>
+      <c r="H65" t="s">
+        <v>37</v>
+      </c>
+      <c r="I65" t="s">
+        <v>21</v>
+      </c>
+      <c r="N65" t="s">
         <v>339</v>
       </c>
-      <c r="B65" t="s">
-        <v>268</v>
-      </c>
-      <c r="C65" t="s">
-        <v>20</v>
-      </c>
-      <c r="D65" s="1">
-        <v>43774</v>
-      </c>
-      <c r="E65" t="s">
-        <v>26</v>
-      </c>
-      <c r="N65" t="s">
+      <c r="O65" t="s">
         <v>340</v>
       </c>
-      <c r="O65" t="s">
-        <v>341</v>
+      <c r="Q65" t="s">
+        <v>32</v>
       </c>
       <c r="R65" t="s">
         <v>26</v>
@@ -4945,57 +4972,325 @@
         <v>26</v>
       </c>
       <c r="T65">
-        <v>242715514</v>
+        <v>552503776</v>
       </c>
       <c r="U65">
-        <v>553488520</v>
+        <v>246922004</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B66" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C66" t="s">
         <v>34</v>
       </c>
       <c r="D66" s="1">
-        <v>44112</v>
+        <v>36558</v>
       </c>
       <c r="E66" t="s">
         <v>26</v>
       </c>
-      <c r="F66" t="s">
-        <v>323</v>
-      </c>
-      <c r="H66" t="s">
-        <v>37</v>
-      </c>
-      <c r="I66" t="s">
-        <v>21</v>
-      </c>
-      <c r="N66" t="s">
+      <c r="R66" t="s">
+        <v>26</v>
+      </c>
+      <c r="S66" t="s">
+        <v>26</v>
+      </c>
+      <c r="T66">
+        <v>543357761</v>
+      </c>
+      <c r="U66">
+        <v>543357761</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>342</v>
+      </c>
+      <c r="B67" t="s">
+        <v>269</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T67">
+        <v>530376302</v>
+      </c>
+      <c r="U67">
+        <v>530376302</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>343</v>
       </c>
-      <c r="O66" t="s">
+      <c r="B68" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T68">
+        <v>559610656</v>
+      </c>
+      <c r="U68">
+        <v>559610656</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>344</v>
       </c>
-      <c r="Q66" t="s">
-        <v>32</v>
-      </c>
-      <c r="R66" t="s">
-        <v>26</v>
-      </c>
-      <c r="S66" t="s">
-        <v>26</v>
-      </c>
-      <c r="T66">
-        <v>552503776</v>
-      </c>
-      <c r="U66">
-        <v>246922004</v>
+      <c r="B69" t="s">
+        <v>269</v>
+      </c>
+      <c r="C69" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T69">
+        <v>540901838</v>
+      </c>
+      <c r="U69">
+        <v>540901838</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>345</v>
+      </c>
+      <c r="B70" t="s">
+        <v>269</v>
+      </c>
+      <c r="C70" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T70">
+        <v>554246016</v>
+      </c>
+      <c r="U70">
+        <v>541473757</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>346</v>
+      </c>
+      <c r="B71" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T71">
+        <v>256503657</v>
+      </c>
+      <c r="U71">
+        <v>256503657</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>347</v>
+      </c>
+      <c r="B72" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T72">
+        <v>240256100</v>
+      </c>
+      <c r="U72">
+        <v>240256100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>348</v>
+      </c>
+      <c r="B73" t="s">
+        <v>318</v>
+      </c>
+      <c r="C73" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T73">
+        <v>240256100</v>
+      </c>
+      <c r="U73">
+        <v>240256100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>349</v>
+      </c>
+      <c r="B74" t="s">
+        <v>268</v>
+      </c>
+      <c r="C74" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T74">
+        <v>557544883</v>
+      </c>
+      <c r="U74">
+        <v>557544883</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>350</v>
+      </c>
+      <c r="B75" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T75">
+        <v>540750426</v>
+      </c>
+      <c r="U75">
+        <v>540750426</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>351</v>
+      </c>
+      <c r="B76" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" t="s">
+        <v>34</v>
+      </c>
+      <c r="D76" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T76">
+        <v>205669296</v>
+      </c>
+      <c r="U76">
+        <v>205669296</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>352</v>
+      </c>
+      <c r="B77" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T77">
+        <v>246898922</v>
+      </c>
+      <c r="U77">
+        <v>246898922</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>353</v>
+      </c>
+      <c r="B78" t="s">
+        <v>354</v>
+      </c>
+      <c r="C78" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" s="1">
+        <v>36558</v>
+      </c>
+      <c r="T78">
+        <v>246898922</v>
+      </c>
+      <c r="U78">
+        <v>246898922</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>355</v>
+      </c>
+      <c r="B79" t="s">
+        <v>266</v>
+      </c>
+      <c r="C79" t="s">
+        <v>34</v>
+      </c>
+      <c r="D79" s="1">
+        <v>36558</v>
+      </c>
+      <c r="E79" t="s">
+        <v>26</v>
+      </c>
+      <c r="T79">
+        <v>244730682</v>
+      </c>
+      <c r="U79">
+        <v>244730682</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>356</v>
+      </c>
+      <c r="B80" t="s">
+        <v>270</v>
+      </c>
+      <c r="C80" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="1">
+        <v>36558</v>
+      </c>
+      <c r="E80" t="s">
+        <v>26</v>
+      </c>
+      <c r="T80">
+        <v>546312435</v>
+      </c>
+      <c r="U80">
+        <v>546312435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>